<commit_message>
Finalizei a aula 2
</commit_message>
<xml_diff>
--- a/Excel VBA/Aula 2 - Formatando Passo a Passo/Produtos.xlsx
+++ b/Excel VBA/Aula 2 - Formatando Passo a Passo/Produtos.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Users\bruno\Documents\GitHub\Alura\Excel VBA\Aula 1 - Organizando a Planilha e Digitando Dados\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Users\bruno\Documents\GitHub\Alura\Excel VBA\Aula 2 - Formatando Passo a Passo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0AC3EAE-A0D4-4A0E-8C35-D66057993AD1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B927A2F-5002-460D-997E-51B89ECFA28F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{F429CDF2-33A2-4A6E-9034-27FA88637C5A}"/>
   </bookViews>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="9">
-  <si>
-    <t>Produtos</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="12">
   <si>
     <t>Tênis Infantil Vermelho</t>
   </si>
@@ -52,13 +49,28 @@
   </si>
   <si>
     <t>Tamanho</t>
+  </si>
+  <si>
+    <t>Lista de Produtos</t>
+  </si>
+  <si>
+    <t>Descrição</t>
+  </si>
+  <si>
+    <t>Preço</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -67,9 +79,37 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFFFF00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <u/>
+      <sz val="16"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="11"/>
-      <color theme="0"/>
+      <sz val="14"/>
+      <color rgb="FFFFFF00"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -84,18 +124,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor theme="4"/>
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor theme="4" tint="0.79998168889431442"/>
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -104,41 +144,201 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
       </left>
       <right/>
-      <top style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
+      <top style="medium">
+        <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </right>
-      <top style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Moeda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -451,163 +651,241 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A6CF0F7-701F-4AD3-A160-66200CB65652}">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" customWidth="1"/>
+    <col min="1" max="1" width="39.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="12"/>
+    </row>
+    <row r="2" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="B3" s="2">
+        <v>27</v>
+      </c>
+      <c r="C3" s="14">
+        <v>85.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="3">
+        <v>28</v>
+      </c>
+      <c r="C4" s="15">
+        <v>89.9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="3">
+        <v>29</v>
+      </c>
+      <c r="C5" s="15">
+        <v>89.9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B6" s="3">
         <v>27</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="C6" s="14">
+        <v>85.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B7" s="3">
         <v>28</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="C7" s="15">
+        <v>89.9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B8" s="3">
         <v>29</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="C8" s="15">
+        <v>89.9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B9" s="3">
         <v>27</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="C9" s="14">
+        <v>85.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B10" s="3">
         <v>28</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="C10" s="15">
+        <v>89.9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B11" s="3">
         <v>29</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="C11" s="15">
+        <v>89.9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="4">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="B12" s="3">
+        <v>29</v>
+      </c>
+      <c r="C12" s="15">
+        <v>123.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="6">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="B13" s="3">
+        <v>40</v>
+      </c>
+      <c r="C13" s="15">
+        <v>123.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="4">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+      <c r="B14" s="3">
+        <v>41</v>
+      </c>
+      <c r="C14" s="15">
+        <v>123.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="6">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+      <c r="B15" s="3">
+        <v>36</v>
+      </c>
+      <c r="C15" s="15">
+        <v>233.9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="4">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+      <c r="B16" s="3">
+        <v>37</v>
+      </c>
+      <c r="C16" s="15">
+        <v>233.9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="6">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="B17" s="3">
+        <v>38</v>
+      </c>
+      <c r="C17" s="15">
+        <v>233.9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="4">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B15" s="6">
+      <c r="B18" s="3">
+        <v>42</v>
+      </c>
+      <c r="C18" s="15">
+        <v>99.99</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="4">
         <v>37</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16" s="4">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B17" s="6">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B18" s="4">
-        <v>37</v>
+      <c r="C19" s="16">
+        <v>99.99</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" s="17"/>
+      <c r="C20" s="13">
+        <f>SUM(C3:C19)</f>
+        <v>2068.0800000000004</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A20:B20"/>
+  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>